<commit_message>
Slight changes to Top Level GA
Now displaying fitness on graph but largest fitness calculation has a
bug
</commit_message>
<xml_diff>
--- a/PaperWork/TasksCompleteList.xlsx
+++ b/PaperWork/TasksCompleteList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="76">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -30,9 +30,6 @@
     <t>Tested</t>
   </si>
   <si>
-    <t>Top Level: GA attempt 2</t>
-  </si>
-  <si>
     <t>Began</t>
   </si>
   <si>
@@ -61,13 +58,199 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Build Top Level: GA attempt 2</t>
+  </si>
+  <si>
+    <t>Test whole EA</t>
+  </si>
+  <si>
+    <t>SHEET 2</t>
+  </si>
+  <si>
+    <t>GA2 Test Results</t>
+  </si>
+  <si>
+    <t>TEST Set :</t>
+  </si>
+  <si>
+    <t>ID:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     0     1     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     0     0     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     0     1     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     1     0     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     1     1     1</t>
+  </si>
+  <si>
+    <t>Gen 1</t>
+  </si>
+  <si>
+    <t>Gen 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     0     1     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     1     0     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>Gen 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     1     1     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     1     1     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     1     1     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     0     0     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     1     0     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1     1     1     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     0     0     1</t>
+  </si>
+  <si>
+    <t>Gen 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     1     0     0     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen 6 </t>
+  </si>
+  <si>
+    <t>Gen 7</t>
+  </si>
+  <si>
+    <t>1     1     1     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     0     1     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen 9 </t>
+  </si>
+  <si>
+    <t>Gen 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1     1     1     1</t>
+  </si>
+  <si>
+    <t>Conclusion:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Improvements needed: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to put a key onto the graph to distinguish the meaning of both the lines </t>
+  </si>
+  <si>
+    <t>Need to take multiple tests and look at the average</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Reasons for test:</t>
+  </si>
+  <si>
+    <t>Checking Completed EA2</t>
+  </si>
+  <si>
+    <t>Test No. : 1</t>
+  </si>
+  <si>
+    <t>Test the graphical display of fitness each generation</t>
+  </si>
+  <si>
+    <t>key added to graph</t>
+  </si>
+  <si>
+    <t>minimum fitness line added to graph</t>
+  </si>
+  <si>
+    <t>intreasted to see how the minimum fitness changes too</t>
+  </si>
+  <si>
+    <t>Resulting Software improvments:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1     1     0     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     0     1     0     0</t>
+  </si>
+  <si>
+    <t>:Manual averaging calculations for checking</t>
+  </si>
+  <si>
+    <t>:Manual Largest Fitness checking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key: </t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can see that the graph is  mapping correctly the average fitness (blue) </t>
+  </si>
+  <si>
+    <t>But there is a bug with the largest fitness (green) two values are wrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1     0     0     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0     0     0     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0     0     0     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0     0     1     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0     1     0     1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,16 +258,88 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -92,16 +347,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="6" builtinId="10"/>
+    <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -111,6 +433,85 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="10314" t="10558" r="7645" b="8414"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="85725" y="3571875"/>
+          <a:ext cx="10629900" cy="5905500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="7449" t="9631" r="7697" b="8692"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="13401675"/>
+          <a:ext cx="15516226" cy="8401050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,15 +801,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
@@ -422,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -431,7 +832,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -439,7 +840,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -447,7 +848,7 @@
         <v>2.1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>42784</v>
@@ -456,10 +857,10 @@
         <v>42786</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -467,7 +868,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>42786</v>
@@ -476,10 +877,10 @@
         <v>42787</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -487,7 +888,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>42787</v>
@@ -496,10 +897,10 @@
         <v>42788</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -507,19 +908,19 @@
         <v>2.4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>42788</v>
       </c>
       <c r="D7" s="1">
-        <v>42788</v>
+        <v>42789</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -527,7 +928,33 @@
         <v>2.5</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42789</v>
+      </c>
+      <c r="D8" s="1">
+        <v>42789</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2.6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42790</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -537,13 +964,770 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <f>(5+3+4+3)/4</f>
+        <v>3.75</v>
+      </c>
+      <c r="B16" s="8">
+        <f>(6+2+4+4)/4</f>
+        <v>4</v>
+      </c>
+      <c r="C16" s="8">
+        <f>(4+6+5+3)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="D16" s="8">
+        <f>(5+3+5+5)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="E16" s="8">
+        <f>(5+3+4+6)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="F16" s="8">
+        <f>(3+4+6+5)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="G16" s="8">
+        <v>5</v>
+      </c>
+      <c r="H16" s="8">
+        <f>(4+4+4+6)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="I16" s="8">
+        <f>(3+3+3+5)/4</f>
+        <v>3.5</v>
+      </c>
+      <c r="J16" s="8">
+        <f>(2+4+4+2)/4</f>
+        <v>3</v>
+      </c>
+      <c r="L16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9">
+        <v>6</v>
+      </c>
+      <c r="C17" s="8">
+        <v>6</v>
+      </c>
+      <c r="D17" s="8">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8">
+        <v>6</v>
+      </c>
+      <c r="F17" s="8">
+        <v>6</v>
+      </c>
+      <c r="G17" s="8">
+        <v>7</v>
+      </c>
+      <c r="H17" s="8">
+        <v>6</v>
+      </c>
+      <c r="I17" s="8">
+        <v>5</v>
+      </c>
+      <c r="J17" s="8">
+        <v>4</v>
+      </c>
+      <c r="L17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K24" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K25" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K26" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K29" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K30" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" t="s">
+        <v>73</v>
+      </c>
+      <c r="F59" t="s">
+        <v>72</v>
+      </c>
+      <c r="G59" t="s">
+        <v>71</v>
+      </c>
+      <c r="H59" t="s">
+        <v>20</v>
+      </c>
+      <c r="I59" t="s">
+        <v>35</v>
+      </c>
+      <c r="J59" t="s">
+        <v>48</v>
+      </c>
+      <c r="K59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" t="s">
+        <v>63</v>
+      </c>
+      <c r="H60" t="s">
+        <v>40</v>
+      </c>
+      <c r="I60" t="s">
+        <v>28</v>
+      </c>
+      <c r="J60" t="s">
+        <v>28</v>
+      </c>
+      <c r="K60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" t="s">
+        <v>44</v>
+      </c>
+      <c r="F61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61" t="s">
+        <v>22</v>
+      </c>
+      <c r="H61" t="s">
+        <v>34</v>
+      </c>
+      <c r="I61" t="s">
+        <v>23</v>
+      </c>
+      <c r="J61" t="s">
+        <v>33</v>
+      </c>
+      <c r="K61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" t="s">
+        <v>20</v>
+      </c>
+      <c r="H62" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" t="s">
+        <v>20</v>
+      </c>
+      <c r="J62" t="s">
+        <v>38</v>
+      </c>
+      <c r="K62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" t="s">
+        <v>63</v>
+      </c>
+      <c r="C63" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" t="s">
+        <v>32</v>
+      </c>
+      <c r="G63" t="s">
+        <v>33</v>
+      </c>
+      <c r="H63" t="s">
+        <v>27</v>
+      </c>
+      <c r="I63" t="s">
+        <v>32</v>
+      </c>
+      <c r="J63" t="s">
+        <v>40</v>
+      </c>
+      <c r="K63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H64" t="s">
+        <v>21</v>
+      </c>
+      <c r="I64" t="s">
+        <v>20</v>
+      </c>
+      <c r="J64" t="s">
+        <v>63</v>
+      </c>
+      <c r="K64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D66" s="8">
+        <f>(5+5+4+4)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="E66" s="8">
+        <f>(4+4+6+4)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="F66" s="8">
+        <f>(3+5+3+5)/4</f>
+        <v>4</v>
+      </c>
+      <c r="G66" s="8">
+        <f>(4+4+4+4)/4</f>
+        <v>4</v>
+      </c>
+      <c r="H66" s="8">
+        <f>(6+2+3+3)/4</f>
+        <v>3.5</v>
+      </c>
+      <c r="I66" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="J66" s="8">
+        <f>(4+5+3+6)/4</f>
+        <v>4.5</v>
+      </c>
+      <c r="L66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D67" s="9">
+        <v>5</v>
+      </c>
+      <c r="E67" s="8">
+        <v>6</v>
+      </c>
+      <c r="F67" s="8">
+        <v>5</v>
+      </c>
+      <c r="G67" s="8">
+        <v>4</v>
+      </c>
+      <c r="H67" s="9">
+        <v>6</v>
+      </c>
+      <c r="I67" s="9">
+        <v>6</v>
+      </c>
+      <c r="J67" s="8">
+        <v>6</v>
+      </c>
+      <c r="L67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated tests sheet, fixed bug in largest fitness, added min fitness graph
</commit_message>
<xml_diff>
--- a/PaperWork/TasksCompleteList.xlsx
+++ b/PaperWork/TasksCompleteList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="79">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -204,9 +204,6 @@
     <t>Resulting Software improvments:</t>
   </si>
   <si>
-    <t xml:space="preserve">  1     1     0     1</t>
-  </si>
-  <si>
     <t xml:space="preserve">     0     1     0     0</t>
   </si>
   <si>
@@ -244,6 +241,18 @@
   </si>
   <si>
     <t xml:space="preserve"> 0     1     0     1</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Found the cause of the bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bug Fixed with a if statement </t>
   </si>
 </sst>
 </file>
@@ -439,13 +448,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -477,15 +486,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>523876</xdr:colOff>
+      <xdr:colOff>323851</xdr:colOff>
       <xdr:row>113</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -501,8 +510,158 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="13401675"/>
+          <a:off x="104775" y="13287375"/>
           <a:ext cx="15516226" cy="8401050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>226314</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>8239</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="285750" y="22802850"/>
+          <a:ext cx="18285714" cy="10285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>273939</xdr:colOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>27289</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="33299400"/>
+          <a:ext cx="18285714" cy="10285714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect l="13075" t="57693" r="56296" b="23231"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5781675" y="44662725"/>
+          <a:ext cx="5600701" cy="1962150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>781051</xdr:colOff>
+      <xdr:row>247</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:srcRect l="4740" t="45283" r="65100" b="23232"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="142875" y="44100749"/>
+          <a:ext cx="5514976" cy="3238501"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -964,105 +1123,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:M250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="Q62" sqref="Q62"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="L241" sqref="L241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="2:13" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
       <c r="E9" t="s">
         <v>33</v>
       </c>
@@ -1076,130 +1233,130 @@
         <v>33</v>
       </c>
       <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
         <v>37</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>32</v>
       </c>
-      <c r="K9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>27</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>20</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>28</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>31</v>
       </c>
-      <c r="K10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>22</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>20</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>32</v>
       </c>
-      <c r="H11" t="s">
-        <v>33</v>
-      </c>
       <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
         <v>38</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>34</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>40</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>32</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>28</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>20</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>24</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
@@ -1207,51 +1364,51 @@
         <v>33</v>
       </c>
       <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" t="s">
         <v>22</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
       </c>
       <c r="I13" t="s">
         <v>38</v>
       </c>
       <c r="J13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" t="s">
         <v>34</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
       </c>
       <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
         <v>44</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>38</v>
-      </c>
-      <c r="I14" t="s">
-        <v>34</v>
       </c>
       <c r="J14" t="s">
         <v>34</v>
@@ -1259,215 +1416,216 @@
       <c r="K14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
         <f>(5+3+4+3)/4</f>
         <v>3.75</v>
       </c>
-      <c r="B16" s="8">
+      <c r="C16" s="8">
         <f>(6+2+4+4)/4</f>
         <v>4</v>
       </c>
-      <c r="C16" s="8">
+      <c r="D16" s="8">
         <f>(4+6+5+3)/4</f>
         <v>4.5</v>
       </c>
-      <c r="D16" s="8">
+      <c r="E16" s="8">
         <f>(5+3+5+5)/4</f>
         <v>4.5</v>
       </c>
-      <c r="E16" s="8">
+      <c r="F16" s="8">
         <f>(5+3+4+6)/4</f>
         <v>4.5</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G16" s="8">
         <f>(3+4+6+5)/4</f>
         <v>4.5</v>
       </c>
-      <c r="G16" s="8">
+      <c r="H16" s="8">
         <v>5</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="8">
         <f>(4+4+4+6)/4</f>
         <v>4.5</v>
       </c>
-      <c r="I16" s="8">
+      <c r="J16" s="8">
         <f>(3+3+3+5)/4</f>
         <v>3.5</v>
       </c>
-      <c r="J16" s="8">
+      <c r="K16" s="8">
         <f>(2+4+4+2)/4</f>
         <v>3</v>
       </c>
-      <c r="L16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="M16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
         <v>5</v>
       </c>
-      <c r="B17" s="9">
+      <c r="C17" s="9">
         <v>6</v>
       </c>
-      <c r="C17" s="8">
+      <c r="D17" s="8">
         <v>6</v>
       </c>
-      <c r="D17" s="8">
+      <c r="E17" s="8">
         <v>5</v>
-      </c>
-      <c r="E17" s="8">
-        <v>6</v>
       </c>
       <c r="F17" s="8">
         <v>6</v>
       </c>
       <c r="G17" s="8">
+        <v>6</v>
+      </c>
+      <c r="H17" s="8">
         <v>7</v>
       </c>
-      <c r="H17" s="8">
+      <c r="I17" s="8">
         <v>6</v>
       </c>
-      <c r="I17" s="8">
+      <c r="J17" s="8">
         <v>5</v>
       </c>
-      <c r="J17" s="8">
+      <c r="K17" s="8">
         <v>4</v>
       </c>
-      <c r="L17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K20" s="5" t="s">
+      <c r="M17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L20" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K21" t="s">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K24" s="7" t="s">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K25" s="6" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K26" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K27" s="3"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K29" s="7" t="s">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="3"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K30" s="6" t="s">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K31" t="s">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K32" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K34" s="7" t="s">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K35" t="s">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K36" t="s">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="D55" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
+    <row r="57" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="D57" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="E57" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="F57" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F57" s="10" t="s">
+      <c r="G57" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G57" s="10" t="s">
+      <c r="H57" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="10" t="s">
+      <c r="I57" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I57" s="10" t="s">
+      <c r="J57" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J57" s="10" t="s">
+      <c r="K57" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="K57" s="10" t="s">
+      <c r="L57" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>62</v>
-      </c>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E59" t="s">
         <v>73</v>
@@ -1479,45 +1637,45 @@
         <v>71</v>
       </c>
       <c r="H59" t="s">
+        <v>70</v>
+      </c>
+      <c r="I59" t="s">
         <v>20</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>35</v>
       </c>
-      <c r="J59" t="s">
+      <c r="K59" t="s">
         <v>48</v>
       </c>
-      <c r="K59" t="s">
+      <c r="L59" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>34</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>20</v>
       </c>
-      <c r="C60" t="s">
-        <v>33</v>
-      </c>
       <c r="D60" t="s">
         <v>33</v>
       </c>
       <c r="E60" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" t="s">
         <v>27</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>28</v>
       </c>
-      <c r="G60" t="s">
-        <v>63</v>
-      </c>
       <c r="H60" t="s">
+        <v>62</v>
+      </c>
+      <c r="I60" t="s">
         <v>40</v>
-      </c>
-      <c r="I60" t="s">
-        <v>28</v>
       </c>
       <c r="J60" t="s">
         <v>28</v>
@@ -1525,116 +1683,116 @@
       <c r="K60" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="L60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>35</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>38</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>21</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>28</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>44</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>28</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>22</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>34</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>23</v>
       </c>
-      <c r="J61" t="s">
-        <v>33</v>
-      </c>
       <c r="K61" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="L61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
         <v>44</v>
-      </c>
-      <c r="B62" t="s">
-        <v>20</v>
       </c>
       <c r="C62" t="s">
         <v>20</v>
       </c>
       <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" t="s">
         <v>21</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>31</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>22</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>20</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>23</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>20</v>
       </c>
-      <c r="J62" t="s">
+      <c r="K62" t="s">
         <v>38</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>31</v>
       </c>
-      <c r="B63" t="s">
-        <v>63</v>
-      </c>
       <c r="C63" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63" t="s">
         <v>44</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>23</v>
       </c>
-      <c r="E63" t="s">
-        <v>33</v>
-      </c>
       <c r="F63" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" t="s">
         <v>32</v>
       </c>
-      <c r="G63" t="s">
-        <v>33</v>
-      </c>
       <c r="H63" t="s">
+        <v>33</v>
+      </c>
+      <c r="I63" t="s">
         <v>27</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>32</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>40</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>33</v>
-      </c>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>33</v>
       </c>
@@ -1648,80 +1806,156 @@
         <v>33</v>
       </c>
       <c r="F64" t="s">
+        <v>33</v>
+      </c>
+      <c r="G64" t="s">
         <v>35</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>28</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>21</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>20</v>
       </c>
-      <c r="J64" t="s">
-        <v>63</v>
-      </c>
       <c r="K64" t="s">
+        <v>62</v>
+      </c>
+      <c r="L64" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B66" s="8">
+        <f>(4+5+4+4)/4</f>
+        <v>4.25</v>
+      </c>
+      <c r="C66" s="8">
+        <f>(4+4+4+4)/4</f>
+        <v>4</v>
+      </c>
       <c r="D66" s="8">
+        <f>(5+3+5+3)/4</f>
+        <v>4</v>
+      </c>
+      <c r="E66" s="8">
         <f>(5+5+4+4)/4</f>
         <v>4.5</v>
       </c>
-      <c r="E66" s="8">
+      <c r="F66" s="8">
         <f>(4+4+6+4)/4</f>
         <v>4.5</v>
       </c>
-      <c r="F66" s="8">
+      <c r="G66" s="8">
         <f>(3+5+3+5)/4</f>
         <v>4</v>
       </c>
-      <c r="G66" s="8">
+      <c r="H66" s="8">
         <f>(4+4+4+4)/4</f>
         <v>4</v>
       </c>
-      <c r="H66" s="8">
+      <c r="I66" s="8">
         <f>(6+2+3+3)/4</f>
         <v>3.5</v>
       </c>
-      <c r="I66" s="8">
+      <c r="J66" s="8">
         <v>4.5</v>
       </c>
-      <c r="J66" s="8">
+      <c r="K66" s="8">
         <f>(4+5+3+6)/4</f>
         <v>4.5</v>
       </c>
-      <c r="L66" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D67" s="9">
+      <c r="M66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B67" s="9">
         <v>5</v>
       </c>
-      <c r="E67" s="8">
+      <c r="C67" s="8">
+        <v>4</v>
+      </c>
+      <c r="D67" s="8">
+        <v>5</v>
+      </c>
+      <c r="E67" s="9">
+        <v>5</v>
+      </c>
+      <c r="F67" s="8">
         <v>6</v>
       </c>
-      <c r="F67" s="8">
+      <c r="G67" s="8">
         <v>5</v>
       </c>
-      <c r="G67" s="8">
+      <c r="H67" s="8">
         <v>4</v>
-      </c>
-      <c r="H67" s="9">
-        <v>6</v>
       </c>
       <c r="I67" s="9">
         <v>6</v>
       </c>
-      <c r="J67" s="8">
+      <c r="J67" s="9">
         <v>6</v>
       </c>
-      <c r="L67" t="s">
-        <v>65</v>
+      <c r="K67" s="8">
+        <v>6</v>
+      </c>
+      <c r="M67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>75</v>
+      </c>
+      <c r="B116" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>77</v>
+      </c>
+      <c r="B230" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A250" s="10"/>
+      <c r="B250" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C250" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D250" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E250" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F250" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G250" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H250" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I250" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J250" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K250" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L250" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code so it can also run until it finds best fit
</commit_message>
<xml_diff>
--- a/PaperWork/TasksCompleteList.xlsx
+++ b/PaperWork/TasksCompleteList.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MEngProjGit\PaperWork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="85">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -253,12 +258,30 @@
   </si>
   <si>
     <t xml:space="preserve">Bug Fixed with a if statement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intresting result from removing the mutation function </t>
+  </si>
+  <si>
+    <t>1     0     0     1</t>
+  </si>
+  <si>
+    <t>0     1     0     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1     0     1     0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1     1     1     1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,6 +462,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -670,6 +696,43 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>898954</xdr:colOff>
+      <xdr:row>355</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:srcRect l="5262" t="12687" r="54343" b="8230"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638176" y="61455299"/>
+          <a:ext cx="11538378" cy="6353175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -716,7 +779,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -751,7 +814,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M250"/>
+  <dimension ref="A1:M320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="L241" sqref="L241"/>
+    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="L339" sqref="L339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,6 +2021,260 @@
         <v>53</v>
       </c>
     </row>
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>79</v>
+      </c>
+      <c r="B310" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A313" s="10"/>
+      <c r="B313" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C313" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D313" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E313" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F313" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G313" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H313" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I313" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J313" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K313" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="L313" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B315" t="s">
+        <v>81</v>
+      </c>
+      <c r="C315" t="s">
+        <v>82</v>
+      </c>
+      <c r="D315" t="s">
+        <v>83</v>
+      </c>
+      <c r="E315" t="s">
+        <v>84</v>
+      </c>
+      <c r="F315" t="s">
+        <v>84</v>
+      </c>
+      <c r="G315" t="s">
+        <v>84</v>
+      </c>
+      <c r="H315" t="s">
+        <v>48</v>
+      </c>
+      <c r="I315" t="s">
+        <v>43</v>
+      </c>
+      <c r="J315" t="s">
+        <v>84</v>
+      </c>
+      <c r="K315" t="s">
+        <v>84</v>
+      </c>
+      <c r="L315" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B316" t="s">
+        <v>27</v>
+      </c>
+      <c r="C316" t="s">
+        <v>28</v>
+      </c>
+      <c r="D316" t="s">
+        <v>20</v>
+      </c>
+      <c r="E316" t="s">
+        <v>33</v>
+      </c>
+      <c r="F316" t="s">
+        <v>33</v>
+      </c>
+      <c r="G316" t="s">
+        <v>33</v>
+      </c>
+      <c r="H316" t="s">
+        <v>33</v>
+      </c>
+      <c r="I316" t="s">
+        <v>33</v>
+      </c>
+      <c r="J316" t="s">
+        <v>33</v>
+      </c>
+      <c r="K316" t="s">
+        <v>33</v>
+      </c>
+      <c r="L316" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B317" t="s">
+        <v>35</v>
+      </c>
+      <c r="C317" t="s">
+        <v>33</v>
+      </c>
+      <c r="D317" t="s">
+        <v>33</v>
+      </c>
+      <c r="E317" t="s">
+        <v>33</v>
+      </c>
+      <c r="F317" t="s">
+        <v>33</v>
+      </c>
+      <c r="G317" t="s">
+        <v>33</v>
+      </c>
+      <c r="H317" t="s">
+        <v>33</v>
+      </c>
+      <c r="I317" t="s">
+        <v>33</v>
+      </c>
+      <c r="J317" t="s">
+        <v>33</v>
+      </c>
+      <c r="K317" t="s">
+        <v>33</v>
+      </c>
+      <c r="L317" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B318" t="s">
+        <v>20</v>
+      </c>
+      <c r="C318" t="s">
+        <v>20</v>
+      </c>
+      <c r="D318" t="s">
+        <v>20</v>
+      </c>
+      <c r="E318" t="s">
+        <v>33</v>
+      </c>
+      <c r="F318" t="s">
+        <v>33</v>
+      </c>
+      <c r="G318" t="s">
+        <v>33</v>
+      </c>
+      <c r="H318" t="s">
+        <v>33</v>
+      </c>
+      <c r="I318" t="s">
+        <v>33</v>
+      </c>
+      <c r="J318" t="s">
+        <v>33</v>
+      </c>
+      <c r="K318" t="s">
+        <v>33</v>
+      </c>
+      <c r="L318" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B319" t="s">
+        <v>20</v>
+      </c>
+      <c r="C319" t="s">
+        <v>20</v>
+      </c>
+      <c r="D319" t="s">
+        <v>20</v>
+      </c>
+      <c r="E319" t="s">
+        <v>33</v>
+      </c>
+      <c r="F319" t="s">
+        <v>33</v>
+      </c>
+      <c r="G319" t="s">
+        <v>33</v>
+      </c>
+      <c r="H319" t="s">
+        <v>33</v>
+      </c>
+      <c r="I319" t="s">
+        <v>33</v>
+      </c>
+      <c r="J319" t="s">
+        <v>33</v>
+      </c>
+      <c r="K319" t="s">
+        <v>33</v>
+      </c>
+      <c r="L319" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B320" t="s">
+        <v>62</v>
+      </c>
+      <c r="C320" t="s">
+        <v>28</v>
+      </c>
+      <c r="D320" t="s">
+        <v>28</v>
+      </c>
+      <c r="E320" t="s">
+        <v>34</v>
+      </c>
+      <c r="F320" t="s">
+        <v>34</v>
+      </c>
+      <c r="G320" t="s">
+        <v>34</v>
+      </c>
+      <c r="H320" t="s">
+        <v>34</v>
+      </c>
+      <c r="I320" t="s">
+        <v>34</v>
+      </c>
+      <c r="J320" t="s">
+        <v>34</v>
+      </c>
+      <c r="K320" t="s">
+        <v>34</v>
+      </c>
+      <c r="L320" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed fitness - added elitism - now converges and stays on fittest
</commit_message>
<xml_diff>
--- a/PaperWork/TasksCompleteList.xlsx
+++ b/PaperWork/TasksCompleteList.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MEngProjGit\PaperWork\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="89">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -276,12 +271,24 @@
   </si>
   <si>
     <t xml:space="preserve"> 1     1     1     1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major Error found - fitness not converging to the max, implemented elitism to fix </t>
+  </si>
+  <si>
+    <t>2.6.1</t>
+  </si>
+  <si>
+    <t>2.6.2</t>
+  </si>
+  <si>
+    <t>Bug with calculating Largest fitness and locus rangeing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -435,7 +442,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -447,6 +454,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -779,7 +789,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -814,7 +824,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1023,15 +1033,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
@@ -1175,8 +1185,39 @@
       <c r="C9" s="1">
         <v>42790</v>
       </c>
+      <c r="D9" s="1">
+        <v>42791</v>
+      </c>
       <c r="E9" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42792</v>
+      </c>
+      <c r="D10" s="1">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42794</v>
+      </c>
+      <c r="D11" s="1">
+        <v>42795</v>
       </c>
     </row>
   </sheetData>
@@ -1188,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="L339" sqref="L339"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L335" sqref="L335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
trying to fix non sorting dominance
</commit_message>
<xml_diff>
--- a/PaperWork/TasksCompleteList.xlsx
+++ b/PaperWork/TasksCompleteList.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MEngProjGit\PaperWork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="98">
   <si>
     <t xml:space="preserve">No. </t>
   </si>
@@ -283,12 +288,39 @@
   </si>
   <si>
     <t>Bug with calculating Largest fitness and locus rangeing</t>
+  </si>
+  <si>
+    <t>Writing test benches for EA</t>
+  </si>
+  <si>
+    <t>SHEET 3</t>
+  </si>
+  <si>
+    <t>Issue:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using num2bin and bin2num, produces and uses binary representation with no spaces, </t>
+  </si>
+  <si>
+    <t>2.7.1</t>
+  </si>
+  <si>
+    <t>2.7.2</t>
+  </si>
+  <si>
+    <t>automaticaly converting decimal input to binary string representation</t>
+  </si>
+  <si>
+    <t>bug with interger to binary mapping  occurred</t>
+  </si>
+  <si>
+    <t>Turns out need to use float encoding</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -746,6 +778,48 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="51725" t="6446" r="27608" b="-111"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="419100"/>
+          <a:ext cx="5038725" cy="9134475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -789,7 +863,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -824,7 +898,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1033,15 +1107,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="74" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
@@ -1218,6 +1292,44 @@
       </c>
       <c r="D11" s="1">
         <v>42795</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2.7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="1">
+        <v>42797</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="1">
+        <v>42797</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2325,12 +2437,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>